<commit_message>
Commit - 3 (Finished game assets...)
Created all assets and completed main slot machine interface.
</commit_message>
<xml_diff>
--- a/Assignment02-SlotMachine/Assets/images/ImageRecords-Assignment2.xlsx
+++ b/Assignment02-SlotMachine/Assets/images/ImageRecords-Assignment2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>OBJECT</t>
   </si>
@@ -50,10 +50,13 @@
     <t>MainSlotMachine</t>
   </si>
   <si>
-    <t>297 px</t>
-  </si>
-  <si>
-    <t>150.5 px</t>
+    <t>Bet Buttons</t>
+  </si>
+  <si>
+    <t>Other Buttons</t>
+  </si>
+  <si>
+    <t>DisplayTextBox</t>
   </si>
 </sst>
 </file>
@@ -433,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,48 +476,66 @@
     </row>
     <row r="3" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C3" s="1">
-        <v>98</v>
+        <v>150.5</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
+      <c r="B4" s="1">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1">
+        <v>30</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1">
+        <v>35</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>298</v>
+      </c>
+      <c r="C6" s="1">
+        <v>98</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>

</xml_diff>